<commit_message>
folder changes, aligned all test cases
</commit_message>
<xml_diff>
--- a/QA/testcases/TestCaseExeSheet.xlsx
+++ b/QA/testcases/TestCaseExeSheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27435" windowHeight="13230"/>
+    <workbookView windowWidth="27465" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
   <si>
     <t>Module Name</t>
   </si>
@@ -23,6 +23,12 @@
     <t>Test Case Name</t>
   </si>
   <si>
+    <t>CPR</t>
+  </si>
+  <si>
+    <t>PatientApp_Process_ViewInComplete</t>
+  </si>
+  <si>
     <t>FAF\Patient</t>
   </si>
   <si>
@@ -113,20 +119,26 @@
     <t>F_PatientApp_Process_ViewIncomplete</t>
   </si>
   <si>
+    <t>LLS\Patient</t>
+  </si>
+  <si>
     <t>L_Patient_Registration_Validation</t>
   </si>
   <si>
     <t>L_Patient_Registration_Positive_Yes</t>
-  </si>
-  <si>
-    <t>LLS\Patient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -139,10 +151,161 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +318,194 @@
         <bgColor indexed="13"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -164,9 +513,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -176,10 +767,57 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -441,22 +1079,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="40.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -475,447 +1113,233 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B28"/>
+      <selection activeCell="A1" sqref="A1:B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -923,7 +1347,7 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -931,10 +1355,11 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
POE1 combination in CPR phar
</commit_message>
<xml_diff>
--- a/QA/testcases/TestCaseExeSheet.xlsx
+++ b/QA/testcases/TestCaseExeSheet.xlsx
@@ -30,85 +30,85 @@
     <t>Phar_Patient_App_Create_PCase_Positive_Alien</t>
   </si>
   <si>
+    <t>CPR\Patient</t>
+  </si>
+  <si>
+    <t>PatientApp_Process_Positive_PCase</t>
+  </si>
+  <si>
+    <t>Phar_Patient_App_Create__DCasePending</t>
+  </si>
+  <si>
     <t>CPR\Provider</t>
   </si>
   <si>
+    <t>Prov_Patient_App_Create__Denied</t>
+  </si>
+  <si>
+    <t>PantientApplication_Mandatory_fields</t>
+  </si>
+  <si>
+    <t>Phar_Patient_App_Create__Denied</t>
+  </si>
+  <si>
+    <t>Prov_Patient_App_Create__PCase_Positive</t>
+  </si>
+  <si>
+    <t>PatientApp_Process_ViewInComplete</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Phar_Patient_App_Create_PCase_Positive</t>
+  </si>
+  <si>
+    <t>Prov_Patient_App_Save_Back_Front_Navi</t>
+  </si>
+  <si>
+    <t>PatientApp_Process_Create_Provider</t>
+  </si>
+  <si>
+    <t>Phar_Patient_App_Save_Back_Front_Navi</t>
+  </si>
+  <si>
+    <t>Prov_Patient_App_ViewIncomplete</t>
+  </si>
+  <si>
+    <t>PatientApp_Process_FrontBack_Navi</t>
+  </si>
+  <si>
+    <t>Phar_Patient_App_ViewIncomplete</t>
+  </si>
+  <si>
+    <t>Provider_Patient_Mandatory_Fields</t>
+  </si>
+  <si>
+    <t>PatientApp_Process_Pending_DCase</t>
+  </si>
+  <si>
+    <t>Phar_Patient_Mandatory_Fields</t>
+  </si>
+  <si>
+    <t>Prov_Patient_Field_Validation</t>
+  </si>
+  <si>
+    <t>PatientApp_ProcessPreviewEditCancel</t>
+  </si>
+  <si>
+    <t>Phar_Patient_Field_Validation</t>
+  </si>
+  <si>
+    <t>Prov_Patient_App_Create__Provider</t>
+  </si>
+  <si>
+    <t>Phar_Patient_App_Create_Provider</t>
+  </si>
+  <si>
+    <t>Prov_Patient_App_Create__DCase_Positive</t>
+  </si>
+  <si>
     <t>Prov_Patient_App_Create_PCase_Positive_Alien</t>
-  </si>
-  <si>
-    <t>CPR\Patient</t>
-  </si>
-  <si>
-    <t>PatientApp_Process_Positive_PCase</t>
-  </si>
-  <si>
-    <t>Phar_Patient_App_Create__DCasePending</t>
-  </si>
-  <si>
-    <t>Prov_Patient_App_Create__Denied</t>
-  </si>
-  <si>
-    <t>PantientApplication_Mandatory_fields</t>
-  </si>
-  <si>
-    <t>Phar_Patient_App_Create__Denied</t>
-  </si>
-  <si>
-    <t>Prov_Patient_App_Create__PCase_Positive</t>
-  </si>
-  <si>
-    <t>PatientApp_Process_ViewInComplete</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Phar_Patient_App_Create_PCase_Positive</t>
-  </si>
-  <si>
-    <t>Prov_Patient_App_Save_Back_Front_Navi</t>
-  </si>
-  <si>
-    <t>PatientApp_Process_Create_Provider</t>
-  </si>
-  <si>
-    <t>Phar_Patient_App_Save_Back_Front_Navi</t>
-  </si>
-  <si>
-    <t>Prov_Patient_App_ViewIncomplete</t>
-  </si>
-  <si>
-    <t>PatientApp_Process_FrontBack_Navi</t>
-  </si>
-  <si>
-    <t>Phar_Patient_App_ViewIncomplete</t>
-  </si>
-  <si>
-    <t>Provider_Patient_Mandatory_Fields</t>
-  </si>
-  <si>
-    <t>PatientApp_Process_Pending_DCase</t>
-  </si>
-  <si>
-    <t>Phar_Patient_Mandatory_Fields</t>
-  </si>
-  <si>
-    <t>Prov_Patient_Field_Validation</t>
-  </si>
-  <si>
-    <t>PatientApp_ProcessPreviewEditCancel</t>
-  </si>
-  <si>
-    <t>Phar_Patient_Field_Validation</t>
-  </si>
-  <si>
-    <t>Prov_Patient_App_Create__Provider</t>
-  </si>
-  <si>
-    <t>Phar_Patient_App_Create_Provider</t>
-  </si>
-  <si>
-    <t>Prov_Patient_App_Create__DCase_Positive</t>
   </si>
   <si>
     <t>FAF\Patient</t>
@@ -321,8 +321,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -356,13 +356,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -370,9 +363,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -384,8 +377,107 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,14 +491,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -414,90 +498,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -520,6 +520,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -532,7 +586,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,49 +604,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,109 +622,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,13 +738,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,26 +801,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -816,148 +816,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1300,13 +1300,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -1326,14 +1326,6 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1365,157 +1357,157 @@
   <sheetData>
     <row r="1" s="3" customFormat="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="1" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" spans="4:7">
@@ -1523,13 +1515,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="4:7">
@@ -1540,10 +1532,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:1">
@@ -1557,7 +1549,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:3">
@@ -1568,7 +1560,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:3">
@@ -1579,7 +1571,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:3">
@@ -1590,7 +1582,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" s="3" customFormat="1" spans="1:3">
@@ -1601,7 +1593,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="1" spans="1:3">
@@ -1612,7 +1604,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="1" spans="1:3">
@@ -1623,7 +1615,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="1" spans="1:1">
@@ -1642,7 +1634,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>41</v>
@@ -1665,7 +1657,7 @@
         <v>45</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>41</v>
@@ -1688,7 +1680,7 @@
         <v>48</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>41</v>
@@ -1711,7 +1703,7 @@
         <v>51</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>41</v>
@@ -1734,7 +1726,7 @@
         <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>41</v>
@@ -1757,7 +1749,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>41</v>
@@ -1780,7 +1772,7 @@
         <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>41</v>
@@ -1926,7 +1918,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>77</v>
@@ -1934,15 +1926,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>78</v>
@@ -1950,7 +1942,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>79</v>
@@ -1958,7 +1950,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>80</v>
@@ -1966,7 +1958,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>81</v>
@@ -2102,7 +2094,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>96</v>
@@ -2110,7 +2102,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>97</v>
@@ -2118,7 +2110,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
POE2 to provider CPR
</commit_message>
<xml_diff>
--- a/QA/testcases/TestCaseExeSheet.xlsx
+++ b/QA/testcases/TestCaseExeSheet.xlsx
@@ -24,24 +24,24 @@
     <t>Test Case Name</t>
   </si>
   <si>
+    <t>CPR\Provider</t>
+  </si>
+  <si>
+    <t>Prov_Patient_App_Create_PCase_Positive_Alien_POE2</t>
+  </si>
+  <si>
+    <t>CPR\Patient</t>
+  </si>
+  <si>
+    <t>PatientApp_Process_Positive_PCase</t>
+  </si>
+  <si>
     <t>CPR\Pharmacy</t>
   </si>
   <si>
-    <t>Phar_Patient_App_Create_PCase_Positive_Alien</t>
-  </si>
-  <si>
-    <t>CPR\Patient</t>
-  </si>
-  <si>
-    <t>PatientApp_Process_Positive_PCase</t>
-  </si>
-  <si>
     <t>Phar_Patient_App_Create__DCasePending</t>
   </si>
   <si>
-    <t>CPR\Provider</t>
-  </si>
-  <si>
     <t>Prov_Patient_App_Create__Denied</t>
   </si>
   <si>
@@ -108,7 +108,7 @@
     <t>Prov_Patient_App_Create__DCase_Positive</t>
   </si>
   <si>
-    <t>Prov_Patient_App_Create_PCase_Positive_Alien</t>
+    <t>Phar_Patient_App_Create_PCase_Positive_Alien_POE2</t>
   </si>
   <si>
     <t>FAF\Patient</t>
@@ -1303,7 +1303,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="$A3:$XFD3"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1349,7 +1349,7 @@
     <col min="2" max="2" width="58.7142857142857" style="3" customWidth="1"/>
     <col min="3" max="3" width="25.5714285714286" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
-    <col min="5" max="5" width="44.5714285714286" style="3" customWidth="1"/>
+    <col min="5" max="5" width="55.1428571428571" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.8571428571429" style="3" customWidth="1"/>
     <col min="7" max="7" width="43.5714285714286" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9" style="3"/>
@@ -1363,13 +1363,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>8</v>
@@ -1383,13 +1383,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>11</v>
@@ -1406,13 +1406,13 @@
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>15</v>
@@ -1429,13 +1429,13 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>18</v>
@@ -1452,13 +1452,13 @@
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>21</v>
@@ -1475,13 +1475,13 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>24</v>
@@ -1498,13 +1498,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>27</v>
@@ -1512,13 +1512,13 @@
     </row>
     <row r="8" s="3" customFormat="1" spans="4:7">
       <c r="D8" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>29</v>
@@ -1526,15 +1526,21 @@
     </row>
     <row r="9" spans="4:7">
       <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="3" t="s">
+    </row>
+    <row r="10" spans="4:5">
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1878,7 +1884,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>72</v>
@@ -1886,7 +1892,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>73</v>
@@ -1894,7 +1900,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>74</v>
@@ -1902,7 +1908,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>75</v>
@@ -1910,7 +1916,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>76</v>
@@ -1918,7 +1924,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>77</v>
@@ -1926,7 +1932,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>29</v>
@@ -1934,7 +1940,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>78</v>
@@ -1942,7 +1948,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>79</v>
@@ -1950,7 +1956,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>80</v>
@@ -1958,7 +1964,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>81</v>

</xml_diff>